<commit_message>
Add PQ, ramp, limit trafo, variability function of time
</commit_message>
<xml_diff>
--- a/Model_optimization/Time_slots.xlsx
+++ b/Model_optimization/Time_slots.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>OT</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>spv</t>
+  </si>
+  <si>
+    <t>CV_D</t>
+  </si>
+  <si>
+    <t>CV_pv</t>
   </si>
 </sst>
 </file>
@@ -350,15 +356,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,8 +374,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -379,8 +391,14 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -390,8 +408,14 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -401,8 +425,14 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -412,8 +442,14 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -423,8 +459,14 @@
       <c r="C6">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -434,8 +476,14 @@
       <c r="C7">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -445,8 +493,14 @@
       <c r="C8">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0.35</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -456,8 +510,14 @@
       <c r="C9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0.35</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -467,8 +527,14 @@
       <c r="C10">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0.35</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -478,8 +544,14 @@
       <c r="C11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0.35</v>
+      </c>
+      <c r="E11">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -489,8 +561,14 @@
       <c r="C12">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0.3</v>
+      </c>
+      <c r="E12">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -500,8 +578,14 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0.3</v>
+      </c>
+      <c r="E13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -511,8 +595,14 @@
       <c r="C14">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0.3</v>
+      </c>
+      <c r="E14">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -522,8 +612,14 @@
       <c r="C15">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+      <c r="E15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -533,8 +629,14 @@
       <c r="C16">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0.35</v>
+      </c>
+      <c r="E16">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -544,8 +646,14 @@
       <c r="C17">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0.35</v>
+      </c>
+      <c r="E17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -555,8 +663,14 @@
       <c r="C18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0.4</v>
+      </c>
+      <c r="E18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -566,8 +680,14 @@
       <c r="C19">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0.45</v>
+      </c>
+      <c r="E19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -577,8 +697,14 @@
       <c r="C20">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -588,8 +714,14 @@
       <c r="C21">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -599,8 +731,14 @@
       <c r="C22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -610,8 +748,14 @@
       <c r="C23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>0.4</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -621,8 +765,14 @@
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0.3</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -630,6 +780,12 @@
         <v>0.53425654320000004</v>
       </c>
       <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.3</v>
+      </c>
+      <c r="E25">
         <v>0</v>
       </c>
     </row>

</xml_diff>